<commit_message>
[1523 zvnl] vóór sein debuggen
</commit_message>
<xml_diff>
--- a/zvnl-9697.xlsx
+++ b/zvnl-9697.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0D6518-65F2-4CEE-97E9-5F530DC3CA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B981587D-037D-42C0-A313-2E4D95530564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7530" yWindow="5797" windowWidth="15247" windowHeight="11648" xr2:uid="{0F794ACE-90AD-42D1-B7AE-7643A8A1DCCD}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="15247" windowHeight="11647" xr2:uid="{0F794ACE-90AD-42D1-B7AE-7643A8A1DCCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Naam</t>
   </si>
@@ -132,6 +132,15 @@
 [n] 2723 &lt;?
 Tabel 28b:
 [x] 5226</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>43568 Ehv</t>
+  </si>
+  <si>
+    <t>Geen</t>
   </si>
 </sst>
 </file>
@@ -187,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -199,6 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -515,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79279987-921F-4756-9C2D-CB9DC226B158}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -537,6 +547,9 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -580,19 +593,27 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
@@ -603,33 +624,38 @@
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B15" s="5"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B19" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>